<commit_message>
completed coding shape, triangle and tests of triangle
</commit_message>
<xml_diff>
--- a/tests/shape/test_plan_triangle.xlsx
+++ b/tests/shape/test_plan_triangle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\8. Activities\Module_02\given_files\activity_2\activity_2\tests\shape\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ADD\Term2\intermediate_software_development\activities\activity_2\tests\shape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82F31A6-8AFA-4B46-AE54-0E71FA70719A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2F0B61-EA5E-4492-9D19-81948509A1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="293" yWindow="0" windowWidth="18240" windowHeight="12480" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -249,13 +249,40 @@
   </si>
   <si>
     <t>calculate_perimeter</t>
+  </si>
+  <si>
+    <t>The triangel instance is created successfully with the attributes correctly set.</t>
+  </si>
+  <si>
+    <t>color = "red",                                                         side_1 = 3,                                                            side_2 = 4,                                                                         side_3 = 5</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>color = "  ",                                                         side_1 = 3,                                                            side_2 = 4,                                                                         side_3 = 5</t>
+  </si>
+  <si>
+    <t>ValueError</t>
+  </si>
+  <si>
+    <t>color = "red",                                                         side_1 = None,                                                            side_2 = 4,                                                                         side_3 = 5</t>
+  </si>
+  <si>
+    <t>color = "red",                                                         side_1 = 3,                                                            side_2 = None,                                                                         side_3 = 5</t>
+  </si>
+  <si>
+    <t>color = "red",                                                         side_1 = 3,                                                            side_2 = 4,                                                                         side_3 = None</t>
+  </si>
+  <si>
+    <t>"The shape color is red.\nThis triangle has three sides with lengths of 3, 4 and 5 centimeters."</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +343,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -503,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -517,9 +560,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -552,6 +592,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1109,53 +1155,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.73046875" customWidth="1"/>
+    <col min="3" max="3" width="22.265625" customWidth="1"/>
+    <col min="4" max="4" width="32.73046875" customWidth="1"/>
+    <col min="5" max="5" width="29.1328125" customWidth="1"/>
+    <col min="6" max="6" width="35.3984375" customWidth="1"/>
+    <col min="7" max="7" width="26.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="2.85">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1175,82 +1221,112 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>2</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>3</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>4</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
+      <c r="E10" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="11">
         <v>5</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12">
+      <c r="E11" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="11">
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1259,12 +1335,18 @@
       <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="11">
+      <c r="E12" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="10">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1273,12 +1355,18 @@
       <c r="D13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11">
+      <c r="E13" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="10">
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1287,32 +1375,38 @@
       <c r="D14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12">
+      <c r="E14" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="11">
         <v>9</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12">
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+    </row>
+    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="11">
         <v>10</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="11">
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+    </row>
+    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="10">
         <v>11</v>
       </c>
       <c r="C17" s="3"/>
@@ -1321,8 +1415,8 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12">
+    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="11">
         <v>12</v>
       </c>
       <c r="C18" s="3"/>
@@ -1331,8 +1425,8 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="12">
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="11">
         <v>13</v>
       </c>
       <c r="C19" s="3"/>
@@ -1341,8 +1435,8 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="11">
+    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="10">
         <v>14</v>
       </c>
       <c r="C20" s="3"/>
@@ -1351,8 +1445,8 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="11">
+    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="10">
         <v>15</v>
       </c>
       <c r="C21" s="3"/>
@@ -1361,8 +1455,8 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="12">
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="11">
         <v>16</v>
       </c>
       <c r="C22" s="3"/>
@@ -1371,8 +1465,8 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="12">
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="11">
         <v>17</v>
       </c>
       <c r="C23" s="3"/>
@@ -1381,8 +1475,8 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="11">
+    <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="10">
         <v>18</v>
       </c>
       <c r="C24" s="3"/>
@@ -1391,15 +1485,15 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="19" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>